<commit_message>
finalyze cometition at ELT
</commit_message>
<xml_diff>
--- a/TetrapolGtw.xlsx
+++ b/TetrapolGtw.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="22590" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Dev" sheetId="1" r:id="rId1"/>
     <sheet name="Tests" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BDD test" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dev!$B$1:$F$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dev!$B$1:$G$90</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="362">
   <si>
     <t>Date</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Markup</t>
-  </si>
-  <si>
-    <t>change creole to other</t>
   </si>
   <si>
     <t>Tags</t>
@@ -629,9 +626,6 @@
     <t>with rating</t>
   </si>
   <si>
-    <t>Comments to be controlled if only raating</t>
-  </si>
-  <si>
     <t>Competition info</t>
   </si>
   <si>
@@ -648,13 +642,595 @@
   </si>
   <si>
     <t>check that tag is not in the list, remove page from the cache</t>
+  </si>
+  <si>
+    <t>create page</t>
+  </si>
+  <si>
+    <t>remonter la coche "page reservée aux administrateurs"</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user1@explik.fr</t>
+  </si>
+  <si>
+    <t>uuuuuuuuuu</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user2@explik.fr</t>
+  </si>
+  <si>
+    <t>user3@explik.fr</t>
+  </si>
+  <si>
+    <t>user4@explik.fr</t>
+  </si>
+  <si>
+    <t>user5@explik.fr</t>
+  </si>
+  <si>
+    <t>control1</t>
+  </si>
+  <si>
+    <t>control2</t>
+  </si>
+  <si>
+    <t>control1@explik.fr</t>
+  </si>
+  <si>
+    <t>control2@explik.fr</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>admin@explik.fr</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>état</t>
+  </si>
+  <si>
+    <t>draft</t>
+  </si>
+  <si>
+    <t>user1 titre1 math draft</t>
+  </si>
+  <si>
+    <t>wysywyg</t>
+  </si>
+  <si>
+    <t>quand on a formatéé un titre, on le sait pas en se positionant dessus ('H' non activé)</t>
+  </si>
+  <si>
+    <t>user1 titre2 architecture soumis</t>
+  </si>
+  <si>
+    <t>architecture</t>
+  </si>
+  <si>
+    <t>soumis</t>
+  </si>
+  <si>
+    <t>les Hx n'ont pas une taille appropriée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags  </t>
+  </si>
+  <si>
+    <t>saisie d'un nouveau tag + entrée</t>
+  </si>
+  <si>
+    <t>active le bouton "valider" de la page</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvaise font </t>
+  </si>
+  <si>
+    <t>user1 titre3 physique headers</t>
+  </si>
+  <si>
+    <t>physique, headers</t>
+  </si>
+  <si>
+    <t>validé</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>&lt;/&gt; inline code ne marche pas</t>
+  </si>
+  <si>
+    <t>à supprimer !!</t>
+  </si>
+  <si>
+    <t>limit code block to youtube</t>
+  </si>
+  <si>
+    <t>control1 titre manger</t>
+  </si>
+  <si>
+    <t>pomme</t>
+  </si>
+  <si>
+    <t>user2 titre 1 tableau</t>
+  </si>
+  <si>
+    <t>histoire tableau</t>
+  </si>
+  <si>
+    <t>user2 titre 2 robot</t>
+  </si>
+  <si>
+    <t>histoire robot</t>
+  </si>
+  <si>
+    <t>user3 titre 1 voiture</t>
+  </si>
+  <si>
+    <t>user3 titre 2 voiture mazda</t>
+  </si>
+  <si>
+    <t>voiture mazda</t>
+  </si>
+  <si>
+    <t>user3 voiture bmw</t>
+  </si>
+  <si>
+    <t>user3 voiture Citroen</t>
+  </si>
+  <si>
+    <t>user3 voiture DS</t>
+  </si>
+  <si>
+    <t>user3 voiture Ford</t>
+  </si>
+  <si>
+    <t>user3 voiture Nissan</t>
+  </si>
+  <si>
+    <t>voiture</t>
+  </si>
+  <si>
+    <t>user3 voiture Peugeot</t>
+  </si>
+  <si>
+    <t>voiture Peugeot</t>
+  </si>
+  <si>
+    <t>user3 voiture Renault</t>
+  </si>
+  <si>
+    <t>voiture Renault</t>
+  </si>
+  <si>
+    <t>user3 voiture Seat</t>
+  </si>
+  <si>
+    <t>voiture Seat</t>
+  </si>
+  <si>
+    <t>user3 voiture Toyota</t>
+  </si>
+  <si>
+    <t>voiture Toyota</t>
+  </si>
+  <si>
+    <t>voiture BMW</t>
+  </si>
+  <si>
+    <t>voiture Citroen</t>
+  </si>
+  <si>
+    <t>voiture DS</t>
+  </si>
+  <si>
+    <t>voiture Ford</t>
+  </si>
+  <si>
+    <t>voiture Nissan</t>
+  </si>
+  <si>
+    <t>commentaires</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>cible</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>robot</t>
+  </si>
+  <si>
+    <t>validation commentaire</t>
+  </si>
+  <si>
+    <t>ajouter titre de la page +  lien vers la page</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>rien</t>
+  </si>
+  <si>
+    <t>nimporte quoi</t>
+  </si>
+  <si>
+    <t>page consultation</t>
+  </si>
+  <si>
+    <t>add a big line between my comments and all comments</t>
+  </si>
+  <si>
+    <t>Alertes</t>
+  </si>
+  <si>
+    <t>motif</t>
+  </si>
+  <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>irrespectueux</t>
+  </si>
+  <si>
+    <t>Citroen</t>
+  </si>
+  <si>
+    <t>polémique</t>
+  </si>
+  <si>
+    <t>list Alerts</t>
+  </si>
+  <si>
+    <t>click on page link</t>
+  </si>
+  <si>
+    <t>error "recontrolepage", srating</t>
+  </si>
+  <si>
+    <t>re-order the menus</t>
+  </si>
+  <si>
+    <t>Concours de voiture</t>
+  </si>
+  <si>
+    <t>__Competition_191007.024815</t>
+  </si>
+  <si>
+    <t>concours</t>
+  </si>
+  <si>
+    <t>la coche "participation" n'existe plus dans la creation de page</t>
+  </si>
+  <si>
+    <t>user1 concours voiture</t>
+  </si>
+  <si>
+    <t>voiture dacia</t>
+  </si>
+  <si>
+    <t>user2 concours voiture</t>
+  </si>
+  <si>
+    <t>voiture ferrari</t>
+  </si>
+  <si>
+    <t>champ pour proposition d'améliorations</t>
+  </si>
+  <si>
+    <t>adapter le message selon que la page est draft ou soumise</t>
+  </si>
+  <si>
+    <t>user3 concours voiture</t>
+  </si>
+  <si>
+    <t>voiture honda</t>
+  </si>
+  <si>
+    <t>user4 concours voiture</t>
+  </si>
+  <si>
+    <t>voiture chrysler</t>
+  </si>
+  <si>
+    <t>user5 concours voiture</t>
+  </si>
+  <si>
+    <t>voiture mitsubishi</t>
+  </si>
+  <si>
+    <t>competitionpage</t>
+  </si>
+  <si>
+    <t>un inscris n'a pas le menu concours</t>
+  </si>
+  <si>
+    <t>notation</t>
+  </si>
+  <si>
+    <t>ferrari</t>
+  </si>
+  <si>
+    <t>chrisler</t>
+  </si>
+  <si>
+    <t>exception when a user rates one of its pages</t>
+  </si>
+  <si>
+    <t>chrysler</t>
+  </si>
+  <si>
+    <t>ferarri</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dump SQL </t>
+  </si>
+  <si>
+    <t>D:\Mes VMWare\SQL Dumps\191008</t>
+  </si>
+  <si>
+    <t>Comments to be controlled if only rating</t>
+  </si>
+  <si>
+    <t>edit page</t>
+  </si>
+  <si>
+    <t>enter on tag leads to an issue</t>
+  </si>
+  <si>
+    <t>les pages de concours dans l'état notation en cours sont affichées dans les dernières publications</t>
+  </si>
+  <si>
+    <t>contrôle page</t>
+  </si>
+  <si>
+    <t>modifier les categories</t>
+  </si>
+  <si>
+    <t>menu contextuel illisible</t>
+  </si>
+  <si>
+    <t>change creole to markdown</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>ma page inscrite au concours</t>
+  </si>
+  <si>
+    <t>menu connexion</t>
+  </si>
+  <si>
+    <t>mettre le focus sur le champ login</t>
+  </si>
+  <si>
+    <t>état draft participation à un concours</t>
+  </si>
+  <si>
+    <t>changer le message : Veuillez soumettre la page pour qu'elle participe au concours"</t>
+  </si>
+  <si>
+    <t>page en draft inscrite à un concours</t>
+  </si>
+  <si>
+    <t>la colonne "concours" est vide</t>
+  </si>
+  <si>
+    <t>MyPages</t>
+  </si>
+  <si>
+    <t>liste</t>
+  </si>
+  <si>
+    <t>remplacer "soumis" par "soumise"</t>
+  </si>
+  <si>
+    <t>low priority</t>
+  </si>
+  <si>
+    <t>Add help modal on click</t>
+  </si>
+  <si>
+    <t>reject page</t>
+  </si>
+  <si>
+    <t>build issue !!!!! With ThemesAvailable</t>
+  </si>
+  <si>
+    <t>registration</t>
+  </si>
+  <si>
+    <t>first registration</t>
+  </si>
+  <si>
+    <t>improve the mail</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>control a page</t>
+  </si>
+  <si>
+    <t>add a [Remove] button to remove the page</t>
+  </si>
+  <si>
+    <t>catégories</t>
+  </si>
+  <si>
+    <t>page en draft</t>
+  </si>
+  <si>
+    <t>les tags de la page en draft s'affichent dans la liste des tags, et la liste des pages est vide !</t>
+  </si>
+  <si>
+    <t>Catégories</t>
+  </si>
+  <si>
+    <t>liste des tags</t>
+  </si>
+  <si>
+    <t>not handled in cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use min files css </t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>will not do</t>
+  </si>
+  <si>
+    <t>can not do</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>Prio</t>
+  </si>
+  <si>
+    <t>Can't do</t>
+  </si>
+  <si>
+    <t>disapeared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page admin </t>
+  </si>
+  <si>
+    <t>première page</t>
+  </si>
+  <si>
+    <t>adapter au markdown ou supprimer</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>modification un tag</t>
+  </si>
+  <si>
+    <t>sites partenaire</t>
+  </si>
+  <si>
+    <t>vérifier les liens</t>
+  </si>
+  <si>
+    <t>page de sites partenaires</t>
+  </si>
+  <si>
+    <t>%managefiles%</t>
+  </si>
+  <si>
+    <t>a supprimer du top menu</t>
+  </si>
+  <si>
+    <t>couleur des titires (H1,H2, …</t>
+  </si>
+  <si>
+    <t>trop foncé !</t>
+  </si>
+  <si>
+    <t>utilisation de l'éditeur du codebloc</t>
+  </si>
+  <si>
+    <t>Ajouter une charte de contenu</t>
+  </si>
+  <si>
+    <t>virer les raisons de rejets</t>
+  </si>
+  <si>
+    <t>indiquer non conforme à la charte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérifier l'affichage des images, en particulier </t>
+  </si>
+  <si>
+    <t>loi offre et demande</t>
+  </si>
+  <si>
+    <t>reject page after control</t>
+  </si>
+  <si>
+    <t>?? Email bof !!</t>
+  </si>
+  <si>
+    <t>Validation des commentaires</t>
+  </si>
+  <si>
+    <t>Ajouter un lien vers la page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,6 +1255,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -722,10 +1306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -754,8 +1339,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1056,11 +1649,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,12 +1661,13 @@
     <col min="1" max="1" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
     <col min="3" max="4" width="40" style="5" customWidth="1"/>
-    <col min="5" max="5" width="60.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="46" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="63.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="46" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,26 +1678,32 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43619</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43619</v>
       </c>
@@ -1114,38 +1714,44 @@
         <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43619</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43619</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43619</v>
       </c>
@@ -1153,13 +1759,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43619</v>
       </c>
@@ -1167,682 +1773,1283 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43619</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="E10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43623</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="E24" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="D25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="E27" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="5" t="s">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="5" t="s">
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43648</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43649</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43649</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="G44" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="5" t="s">
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="5" t="s">
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="5" t="s">
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E48" s="5" t="s">
+    </row>
+    <row r="49" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="G49" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E50" s="5" t="s">
+    </row>
+    <row r="51" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="F52" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="F53" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E54" s="5" t="s">
+    </row>
+    <row r="55" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E55" s="5" t="s">
+    </row>
+    <row r="56" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="F59" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D60" s="5" t="s">
+    </row>
+    <row r="61" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>169</v>
       </c>
+      <c r="G61" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F68" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F69" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F70" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F71" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F74" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43796</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F86" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F87" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F89" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>361</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F56">
+  <autoFilter ref="B1:G90">
     <filterColumn colId="0">
       <filters>
-        <filter val="ToFix"/>
+        <filter val="ToDev"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1856,7 +3063,7 @@
   <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1871,182 +3078,182 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D20" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2057,12 +3264,838 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" t="s">
+        <v>210</v>
+      </c>
+      <c r="F16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" t="s">
+        <v>218</v>
+      </c>
+      <c r="E19" t="s">
+        <v>219</v>
+      </c>
+      <c r="F19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" t="s">
+        <v>275</v>
+      </c>
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" t="s">
+        <v>225</v>
+      </c>
+      <c r="E24" t="s">
+        <v>239</v>
+      </c>
+      <c r="F24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" t="s">
+        <v>240</v>
+      </c>
+      <c r="F25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" t="s">
+        <v>243</v>
+      </c>
+      <c r="F28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" t="s">
+        <v>232</v>
+      </c>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" t="s">
+        <v>234</v>
+      </c>
+      <c r="F30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" t="s">
+        <v>235</v>
+      </c>
+      <c r="E31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F31" t="s">
+        <v>211</v>
+      </c>
+      <c r="H31" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" t="s">
+        <v>237</v>
+      </c>
+      <c r="E32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" t="s">
+        <v>279</v>
+      </c>
+      <c r="F33" t="s">
+        <v>202</v>
+      </c>
+      <c r="H33" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" t="s">
+        <v>280</v>
+      </c>
+      <c r="E35" t="s">
+        <v>281</v>
+      </c>
+      <c r="F35" t="s">
+        <v>211</v>
+      </c>
+      <c r="H35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" t="s">
+        <v>282</v>
+      </c>
+      <c r="E36" t="s">
+        <v>283</v>
+      </c>
+      <c r="F36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>244</v>
+      </c>
+      <c r="C39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D39" t="s">
+        <v>246</v>
+      </c>
+      <c r="E39" t="s">
+        <v>247</v>
+      </c>
+      <c r="G39" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" t="s">
+        <v>248</v>
+      </c>
+      <c r="F40" t="s">
+        <v>211</v>
+      </c>
+      <c r="G40">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" t="s">
+        <v>249</v>
+      </c>
+      <c r="F41" t="s">
+        <v>211</v>
+      </c>
+      <c r="G41" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" t="s">
+        <v>211</v>
+      </c>
+      <c r="G43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>250</v>
+      </c>
+      <c r="F44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>258</v>
+      </c>
+      <c r="C48" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F48" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49" t="s">
+        <v>260</v>
+      </c>
+      <c r="F49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>268</v>
+      </c>
+      <c r="E53" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>284</v>
+      </c>
+      <c r="D57" t="s">
+        <v>247</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>230</v>
+      </c>
+      <c r="D58" t="s">
+        <v>287</v>
+      </c>
+      <c r="E58" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" t="s">
+        <v>288</v>
+      </c>
+      <c r="E59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>230</v>
+      </c>
+      <c r="D60" t="s">
+        <v>291</v>
+      </c>
+      <c r="E60" t="s">
+        <v>178</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" t="s">
+        <v>291</v>
+      </c>
+      <c r="E61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" t="s">
+        <v>290</v>
+      </c>
+      <c r="E62" t="s">
+        <v>176</v>
+      </c>
+      <c r="F62" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63" t="s">
+        <v>287</v>
+      </c>
+      <c r="E63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>230</v>
+      </c>
+      <c r="D64" t="s">
+        <v>291</v>
+      </c>
+      <c r="E64" t="s">
+        <v>172</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>230</v>
+      </c>
+      <c r="D65" t="s">
+        <v>290</v>
+      </c>
+      <c r="E65" t="s">
+        <v>172</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>230</v>
+      </c>
+      <c r="D66" t="s">
+        <v>287</v>
+      </c>
+      <c r="E66" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>230</v>
+      </c>
+      <c r="D67" t="s">
+        <v>291</v>
+      </c>
+      <c r="E67" t="s">
+        <v>175</v>
+      </c>
+      <c r="F67" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>230</v>
+      </c>
+      <c r="D68" t="s">
+        <v>290</v>
+      </c>
+      <c r="E68" t="s">
+        <v>175</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>230</v>
+      </c>
+      <c r="D69" t="s">
+        <v>287</v>
+      </c>
+      <c r="E69" t="s">
+        <v>175</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>293</v>
+      </c>
+      <c r="D71" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add keepalive for edition. Allow rating for all viewers. Various.
</commit_message>
<xml_diff>
--- a/TetrapolGtw.xlsx
+++ b/TetrapolGtw.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDA88C-CC40-4056-908B-F9001E67C213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="22590" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20088" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="365">
   <si>
     <t>Date</t>
   </si>
@@ -1225,11 +1226,20 @@
   <si>
     <t>Ajouter un lien vers la page</t>
   </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Reject a page when controling</t>
+  </si>
+  <si>
+    <t>error after reject !!! Mail ????</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1357,6 +1367,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1404,7 +1417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1437,9 +1450,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1472,6 +1502,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1647,27 +1694,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="5" customWidth="1"/>
     <col min="3" max="4" width="40" style="5" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="63.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="46" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +1737,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43619</v>
       </c>
@@ -1703,7 +1750,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43619</v>
       </c>
@@ -1720,7 +1767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43619</v>
       </c>
@@ -1737,7 +1784,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43619</v>
       </c>
@@ -1751,7 +1798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43619</v>
       </c>
@@ -1765,7 +1812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43619</v>
       </c>
@@ -1779,7 +1826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43619</v>
       </c>
@@ -1796,7 +1843,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1810,7 +1857,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1822,7 +1869,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1834,7 +1881,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1846,7 +1893,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1871,7 +1918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1883,7 +1930,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
@@ -1891,7 +1938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43623</v>
       </c>
@@ -1911,12 +1958,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1930,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1941,7 +1988,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>29</v>
       </c>
@@ -1955,7 +2002,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1969,7 +2016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1983,7 +2030,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>46</v>
       </c>
@@ -1994,7 +2041,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
@@ -2008,7 +2055,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>46</v>
       </c>
@@ -2022,7 +2069,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
@@ -2036,7 +2083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>46</v>
       </c>
@@ -2051,7 +2098,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>46</v>
       </c>
@@ -2066,7 +2113,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
@@ -2081,7 +2128,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>46</v>
       </c>
@@ -2095,7 +2142,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>46</v>
       </c>
@@ -2109,7 +2156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>46</v>
       </c>
@@ -2123,7 +2170,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>46</v>
       </c>
@@ -2137,7 +2184,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>16</v>
       </c>
@@ -2151,7 +2198,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>16</v>
       </c>
@@ -2166,7 +2213,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>3</v>
       </c>
@@ -2183,7 +2230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43648</v>
       </c>
@@ -2203,7 +2250,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>3</v>
       </c>
@@ -2220,9 +2267,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>43649</v>
       </c>
@@ -2233,7 +2280,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43649</v>
       </c>
@@ -2250,7 +2297,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2314,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>16</v>
       </c>
@@ -2281,7 +2328,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>16</v>
       </c>
@@ -2295,7 +2342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2353,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
         <v>16</v>
       </c>
@@ -2320,7 +2367,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>8</v>
       </c>
@@ -2337,7 +2384,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="50" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
         <v>16</v>
       </c>
@@ -2348,7 +2395,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>16</v>
       </c>
@@ -2359,7 +2406,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
         <v>3</v>
       </c>
@@ -2376,7 +2423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2451,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>16</v>
       </c>
@@ -2418,7 +2465,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2479,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>16</v>
       </c>
@@ -2443,7 +2490,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>8</v>
       </c>
@@ -2457,7 +2504,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>16</v>
       </c>
@@ -2488,7 +2535,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
         <v>8</v>
       </c>
@@ -2502,7 +2549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B62" s="5" t="s">
         <v>8</v>
       </c>
@@ -2516,7 +2563,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="63" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63" s="5" t="s">
         <v>8</v>
       </c>
@@ -2530,7 +2577,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="64" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
         <v>8</v>
       </c>
@@ -2547,7 +2594,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
         <v>8</v>
       </c>
@@ -2564,7 +2611,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2625,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B67" s="5" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2636,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B68" s="5" t="s">
         <v>3</v>
       </c>
@@ -2603,7 +2650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B69" s="5" t="s">
         <v>3</v>
       </c>
@@ -2617,7 +2664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" s="5" t="s">
         <v>8</v>
       </c>
@@ -2634,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B71" s="5" t="s">
         <v>3</v>
       </c>
@@ -2645,7 +2692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11"/>
       <c r="B72" s="11" t="s">
         <v>8</v>
@@ -2662,7 +2709,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
         <v>3</v>
       </c>
@@ -2673,7 +2720,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>3</v>
       </c>
@@ -2687,7 +2734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
         <v>8</v>
       </c>
@@ -2701,7 +2748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
         <v>8</v>
       </c>
@@ -2715,7 +2762,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B77" s="5" t="s">
         <v>8</v>
       </c>
@@ -2729,7 +2776,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B78" s="5" t="s">
         <v>8</v>
       </c>
@@ -2743,7 +2790,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B79" s="5" t="s">
         <v>8</v>
       </c>
@@ -2760,7 +2807,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" s="5" t="s">
         <v>3</v>
       </c>
@@ -2777,7 +2824,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B81" s="5" t="s">
         <v>8</v>
       </c>
@@ -2788,7 +2835,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B82" s="5" t="s">
         <v>8</v>
       </c>
@@ -2802,7 +2849,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B83" s="5" t="s">
         <v>8</v>
       </c>
@@ -2819,7 +2866,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B84" s="5" t="s">
         <v>8</v>
       </c>
@@ -2836,7 +2883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>43796</v>
       </c>
@@ -2853,7 +2900,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B86" s="5" t="s">
         <v>3</v>
       </c>
@@ -2870,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
         <v>3</v>
       </c>
@@ -2887,7 +2934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B88" s="5" t="s">
         <v>8</v>
       </c>
@@ -2904,7 +2951,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B89" s="5" t="s">
         <v>8</v>
       </c>
@@ -2921,7 +2968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B90" s="5" t="s">
         <v>3</v>
       </c>
@@ -2929,7 +2976,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B91" s="5" t="s">
         <v>3</v>
       </c>
@@ -2943,7 +2990,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2954,7 +3001,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
         <v>16</v>
       </c>
@@ -2968,7 +3015,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B94" s="5" t="s">
         <v>8</v>
       </c>
@@ -2979,7 +3026,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B95" s="5" t="s">
         <v>8</v>
       </c>
@@ -2990,7 +3037,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B96" s="5" t="s">
         <v>8</v>
       </c>
@@ -2998,7 +3045,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="5" t="s">
         <v>3</v>
       </c>
@@ -3012,7 +3059,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="5" t="s">
         <v>16</v>
       </c>
@@ -3023,7 +3070,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="5" t="s">
         <v>16</v>
       </c>
@@ -3034,7 +3081,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="5" t="s">
         <v>3</v>
       </c>
@@ -3045,8 +3092,22 @@
         <v>361</v>
       </c>
     </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:G90">
+  <autoFilter ref="B1:G90" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="ToDev"/>
@@ -3059,24 +3120,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="6"/>
-    <col min="3" max="3" width="13.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="74.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="2" width="9.109375" style="6"/>
+    <col min="3" max="3" width="13.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="59.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="74.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="65.88671875" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>73</v>
       </c>
@@ -3087,12 +3148,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>74</v>
       </c>
@@ -3109,7 +3170,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
         <v>49</v>
       </c>
@@ -3120,7 +3181,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="6" t="s">
         <v>49</v>
       </c>
@@ -3131,7 +3192,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
         <v>49</v>
       </c>
@@ -3142,7 +3203,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
         <v>85</v>
       </c>
@@ -3153,7 +3214,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
         <v>88</v>
       </c>
@@ -3164,7 +3225,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>95</v>
       </c>
@@ -3175,7 +3236,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="6" t="s">
         <v>91</v>
       </c>
@@ -3183,7 +3244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="6" t="s">
         <v>92</v>
       </c>
@@ -3191,7 +3252,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="6" t="s">
         <v>94</v>
       </c>
@@ -3199,7 +3260,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
         <v>71</v>
       </c>
@@ -3210,7 +3271,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
         <v>49</v>
       </c>
@@ -3221,7 +3282,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="6" t="s">
         <v>98</v>
       </c>
@@ -3232,7 +3293,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="6" t="s">
         <v>100</v>
       </c>
@@ -3243,7 +3304,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D19" s="6" t="s">
         <v>103</v>
       </c>
@@ -3251,7 +3312,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D20" s="6" t="s">
         <v>89</v>
       </c>
@@ -3263,20 +3324,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H71"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>170</v>
       </c>
@@ -3290,7 +3351,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>170</v>
       </c>
@@ -3301,7 +3362,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>172</v>
       </c>
@@ -3312,7 +3373,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>175</v>
       </c>
@@ -3323,7 +3384,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>178</v>
       </c>
@@ -3334,7 +3395,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>176</v>
       </c>
@@ -3345,7 +3406,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>177</v>
       </c>
@@ -3356,7 +3417,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>183</v>
       </c>
@@ -3367,7 +3428,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>184</v>
       </c>
@@ -3378,7 +3439,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>187</v>
       </c>
@@ -3401,7 +3462,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>172</v>
       </c>
@@ -3415,7 +3476,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>172</v>
       </c>
@@ -3429,7 +3490,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>172</v>
       </c>
@@ -3446,7 +3507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>172</v>
       </c>
@@ -3463,7 +3524,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>183</v>
       </c>
@@ -3477,7 +3538,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>175</v>
       </c>
@@ -3491,7 +3552,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>175</v>
       </c>
@@ -3505,7 +3566,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>175</v>
       </c>
@@ -3522,7 +3583,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>178</v>
       </c>
@@ -3536,7 +3597,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>178</v>
       </c>
@@ -3550,7 +3611,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>178</v>
       </c>
@@ -3564,7 +3625,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>178</v>
       </c>
@@ -3578,7 +3639,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>178</v>
       </c>
@@ -3592,7 +3653,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>178</v>
       </c>
@@ -3606,7 +3667,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>178</v>
       </c>
@@ -3620,7 +3681,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>178</v>
       </c>
@@ -3634,7 +3695,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>178</v>
       </c>
@@ -3648,7 +3709,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>178</v>
       </c>
@@ -3665,7 +3726,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>178</v>
       </c>
@@ -3679,7 +3740,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>178</v>
       </c>
@@ -3696,7 +3757,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>171</v>
       </c>
@@ -3707,7 +3768,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>176</v>
       </c>
@@ -3724,7 +3785,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>177</v>
       </c>
@@ -3741,7 +3802,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>244</v>
       </c>
@@ -3758,7 +3819,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>175</v>
       </c>
@@ -3775,7 +3836,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>175</v>
       </c>
@@ -3792,7 +3853,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>176</v>
       </c>
@@ -3806,7 +3867,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>176</v>
       </c>
@@ -3823,7 +3884,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>176</v>
       </c>
@@ -3837,7 +3898,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>258</v>
       </c>
@@ -3854,7 +3915,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>177</v>
       </c>
@@ -3868,7 +3929,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>177</v>
       </c>
@@ -3882,12 +3943,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>268</v>
       </c>
@@ -3895,7 +3956,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>284</v>
       </c>
@@ -3909,7 +3970,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>230</v>
       </c>
@@ -3923,7 +3984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>230</v>
       </c>
@@ -3937,7 +3998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
         <v>230</v>
       </c>
@@ -3951,7 +4012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>230</v>
       </c>
@@ -3965,7 +4026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>230</v>
       </c>
@@ -3979,7 +4040,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>230</v>
       </c>
@@ -3993,7 +4054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
         <v>230</v>
       </c>
@@ -4007,7 +4068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>230</v>
       </c>
@@ -4021,7 +4082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>230</v>
       </c>
@@ -4035,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>230</v>
       </c>
@@ -4049,7 +4110,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>230</v>
       </c>
@@ -4063,7 +4124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>230</v>
       </c>
@@ -4077,7 +4138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>293</v>
       </c>
@@ -4087,14 +4148,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="D2" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>